<commit_message>
Hook can drag things around, added hook pivot
Hook attaches to any hookable object and can pull lighter things towards
Narissa. Heavier objects are harder to pull and will cause Narissa to
pull herself towards the object instead.
</commit_message>
<xml_diff>
--- a/Documents/Personal files/HP/Tidsrapport HP v15.xlsx
+++ b/Documents/Personal files/HP/Tidsrapport HP v15.xlsx
@@ -190,22 +190,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,12 +526,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -540,50 +540,50 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="19">
-        <v>14</v>
-      </c>
-      <c r="C3" s="19"/>
+      <c r="B3" s="15">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
@@ -636,8 +636,8 @@
       <c r="A13" s="11">
         <v>42104</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -949,6 +949,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
@@ -957,12 +963,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>